<commit_message>
- ADD: Added template for geotiff trials images.
- CHG: Updated trials template to latest version.
</commit_message>
<xml_diff>
--- a/trials-data/trials-data.xlsx
+++ b/trials-data/trials-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sr41756\workspaces\misc\germinate-data-templates\trials-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34629FCB-7AF0-40ED-8D89-9823A35D2A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CD3032-92FE-4E67-BDD9-F1701119FD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="117">
   <si>
     <t>Name</t>
   </si>
@@ -399,6 +399,12 @@
   </si>
   <si>
     <t>Please include any additional information that details how this experiment was carried out in a text or Word document and send along with this template. If there are any images please send these as individual JPG files. Mandatory fields are highlighted in yellow.</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Column</t>
   </si>
 </sst>
 </file>
@@ -607,6 +613,27 @@
   </cellStyles>
   <dxfs count="27">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="yyyymmdd"/>
     </dxf>
     <dxf>
@@ -689,20 +716,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -798,13 +811,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -845,29 +851,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CDFAA9A6-0123-422D-B80F-81EB2270DAA0}" name="Table7" displayName="Table7" ref="A1:C18" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CDFAA9A6-0123-422D-B80F-81EB2270DAA0}" name="Table7" displayName="Table7" ref="A1:C18" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A1:C18" xr:uid="{DCA4608A-E2D9-45F1-81E3-F49396F38526}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1E03C996-7263-422B-8AA0-13669C78161F}" name="LABEL" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{A20F043F-90CD-41BB-866B-522B95F3EC18}" name="DEFINITION" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{139364FF-5D24-40BF-A84C-CF209A3E5D65}" name="VALUE" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{1E03C996-7263-422B-8AA0-13669C78161F}" name="LABEL" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{A20F043F-90CD-41BB-866B-522B95F3EC18}" name="DEFINITION" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{139364FF-5D24-40BF-A84C-CF209A3E5D65}" name="VALUE" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:L12" totalsRowShown="0">
-  <autoFilter ref="A1:L12" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:N12" totalsRowShown="0">
+  <autoFilter ref="A1:N12" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Line/Phenotype"/>
     <tableColumn id="2" xr3:uid="{CB956365-108C-47D3-B28E-EBDFD6E16995}" name="Rep"/>
     <tableColumn id="9" xr3:uid="{8C52E70E-74F2-424A-8F55-980BEB83541C}" name="Block"/>
+    <tableColumn id="13" xr3:uid="{20544D5A-2E37-40C0-8903-7DFE8E1801E4}" name="Row"/>
+    <tableColumn id="14" xr3:uid="{CE255CEA-3127-418C-9432-3F63F51FD781}" name="Column"/>
     <tableColumn id="7" xr3:uid="{88B30358-C3FE-4E11-B08D-42FB21CD6479}" name="Treatment"/>
     <tableColumn id="8" xr3:uid="{13CC7C54-6C19-41EF-BA0D-75E84678E993}" name="Location"/>
-    <tableColumn id="10" xr3:uid="{4DB6F789-093F-4C73-B982-C2E54070E165}" name="Latitude" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{7DF6B222-3988-4F46-991B-F6C2F213B41D}" name="Longitude" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{55ED41BA-9315-4A55-B989-C3614B9C3340}" name="Elevation" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{4DB6F789-093F-4C73-B982-C2E54070E165}" name="Latitude" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{7DF6B222-3988-4F46-991B-F6C2F213B41D}" name="Longitude" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{55ED41BA-9315-4A55-B989-C3614B9C3340}" name="Elevation" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Ear length"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Ear number per plant"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Ear width"/>
@@ -889,9 +897,9 @@
     <tableColumn id="11" xr3:uid="{907497DD-05CD-436D-8F9D-C9733135B6D1}" name="Latitude"/>
     <tableColumn id="10" xr3:uid="{F68843F4-17C8-471E-8FEA-8A1CF9BD7F9F}" name="Longitude"/>
     <tableColumn id="9" xr3:uid="{97B62C49-64CB-4474-93B9-41298499FF28}" name="Elevation"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Ear length" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Ear number per plant" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Ear width" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Ear length" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Ear number per plant" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Ear width" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -917,12 +925,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{22E566EA-CF41-4BD4-A877-BF1A04CBE27C}" name="Table47" displayName="Table47" ref="A1:H2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:H2" xr:uid="{C24E8378-3794-454E-84CF-B08C2B5A27D2}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{22E566EA-CF41-4BD4-A877-BF1A04CBE27C}" name="Table47" displayName="Table47" ref="A1:J2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:J2" xr:uid="{C24E8378-3794-454E-84CF-B08C2B5A27D2}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{CCD80E05-5388-423E-BBDC-2354AB7B8FC3}" name="Line/Phenotype"/>
     <tableColumn id="2" xr3:uid="{466AEB02-1AD0-430A-B6D8-FF71A9F751B4}" name="Rep"/>
     <tableColumn id="8" xr3:uid="{B32A4B56-1C05-4F7B-B51B-4FA3967354E2}" name="Block"/>
+    <tableColumn id="9" xr3:uid="{2ED92832-AD7D-4A22-8917-F561E101C555}" name="Row"/>
+    <tableColumn id="10" xr3:uid="{61C248C8-9EF3-432C-BE20-51527617EB5B}" name="Column"/>
     <tableColumn id="7" xr3:uid="{40C0F606-B99C-4595-806C-A7295CC796D9}" name="Treatment"/>
     <tableColumn id="3" xr3:uid="{8EE9A1A1-AEF3-490F-B2E4-D6A460210A54}" name="Location"/>
     <tableColumn id="4" xr3:uid="{69C9CE63-BD11-4E4B-957D-A99D3AA2F63C}" name="Latitude"/>
@@ -934,12 +944,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E4E9D794-B34F-44CE-84F6-AA0D14CDB5C6}" name="Table4411" displayName="Table4411" ref="A1:H2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:H2" xr:uid="{7A5E0959-3CB3-48DB-A1FB-2A58B80F3191}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E4E9D794-B34F-44CE-84F6-AA0D14CDB5C6}" name="Table4411" displayName="Table4411" ref="A1:J2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:J2" xr:uid="{7A5E0959-3CB3-48DB-A1FB-2A58B80F3191}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{4C72BB57-561C-4C97-9A88-82A2D428A82A}" name="Line/Phenotype"/>
     <tableColumn id="7" xr3:uid="{D9EE74B9-83DA-4C06-B461-5A4F7DC2FD15}" name="Rep"/>
     <tableColumn id="4" xr3:uid="{57727AAB-E4BF-42AD-962C-0DBC24A599A0}" name="Block"/>
+    <tableColumn id="9" xr3:uid="{01A0EDA9-30E9-4526-A528-8A71ADD7B449}" name="Row"/>
+    <tableColumn id="10" xr3:uid="{C40DC8EF-6D3A-43F0-B3FC-4A7CF45DCFE4}" name="Column"/>
     <tableColumn id="2" xr3:uid="{233E7CDA-E23F-4F59-95B7-C14E55E139E2}" name="Treatment"/>
     <tableColumn id="3" xr3:uid="{9976F5CF-934C-4F0C-8E8C-314FBD437428}" name="Location"/>
     <tableColumn id="5" xr3:uid="{2F3B018F-D870-41DE-A4AF-30757F61E6A4}" name="Latitude"/>
@@ -963,18 +975,18 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{35BDF020-ABCA-4439-B958-8014090B32CC}" name="Table8" displayName="Table8" ref="A1:I2" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{35BDF020-ABCA-4439-B958-8014090B32CC}" name="Table8" displayName="Table8" ref="A1:I2" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:I2" xr:uid="{1B38FBA2-DC2A-4EE8-9782-869C402F129F}"/>
   <tableColumns count="9">
-    <tableColumn id="2" xr3:uid="{11A585B5-EAF2-4086-9D85-0D60A53887C4}" name="Last Name" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{4077ACA3-84ED-4981-AB4E-365AEBA76825}" name="First Name" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{B35B0A33-6132-493B-9131-6BA92C731A13}" name="Contributor role" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{901F3798-43D3-40F0-8C23-0793303EE87C}" name="Contributor ID" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{0A90BD52-57A6-4CDE-BA8E-5136E8A1EAB8}" name="Email" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{03F1C9C1-7B2C-4F0C-B099-1F465D301B93}" name="Phone" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{65BCBC93-FC74-4E14-B6A5-BF465AB5D91D}" name="Contributor" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{5C332E95-780E-414E-B1E2-86318BE35F31}" name="Address" dataDxfId="7"/>
-    <tableColumn id="1" xr3:uid="{9A8DCFA6-0AF2-4BA7-95EB-E0D0FE3A6153}" name="Country" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{11A585B5-EAF2-4086-9D85-0D60A53887C4}" name="Last Name" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{4077ACA3-84ED-4981-AB4E-365AEBA76825}" name="First Name" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{B35B0A33-6132-493B-9131-6BA92C731A13}" name="Contributor role" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{901F3798-43D3-40F0-8C23-0793303EE87C}" name="Contributor ID" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{0A90BD52-57A6-4CDE-BA8E-5136E8A1EAB8}" name="Email" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{03F1C9C1-7B2C-4F0C-B099-1F465D301B93}" name="Phone" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{65BCBC93-FC74-4E14-B6A5-BF465AB5D91D}" name="Contributor" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{5C332E95-780E-414E-B1E2-86318BE35F31}" name="Address" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{9A8DCFA6-0AF2-4BA7-95EB-E0D0FE3A6153}" name="Country" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1294,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,7 +1530,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C3">
-    <cfRule type="containsBlanks" dxfId="24" priority="1">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1535,28 +1547,28 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="6.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1567,34 +1579,40 @@
         <v>97</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -1604,35 +1622,41 @@
       <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="4">
+      <c r="H2" s="4">
         <v>56.46152</v>
       </c>
-      <c r="G2" s="4">
+      <c r="I2" s="4">
         <v>-3.1109200000000001</v>
       </c>
-      <c r="H2" s="4">
+      <c r="J2" s="4">
         <v>38.9</v>
       </c>
-      <c r="I2" s="4">
+      <c r="K2" s="4">
         <v>15.698600000000001</v>
       </c>
-      <c r="J2" s="4">
+      <c r="L2" s="4">
         <v>7</v>
       </c>
-      <c r="K2" s="4">
+      <c r="M2" s="4">
         <v>20.435199999999998</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
@@ -1642,35 +1666,41 @@
       <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="4">
+      <c r="H3" s="4">
         <v>56.470471000000003</v>
       </c>
-      <c r="G3" s="4">
+      <c r="I3" s="4">
         <v>-3.1227999999999998</v>
       </c>
-      <c r="H3" s="4">
+      <c r="J3" s="4">
         <v>26.4</v>
       </c>
-      <c r="I3" s="4">
+      <c r="K3" s="4">
         <v>17.075500000000002</v>
       </c>
-      <c r="J3" s="4">
+      <c r="L3" s="4">
         <v>8</v>
       </c>
-      <c r="K3" s="4">
+      <c r="M3" s="4">
         <v>24.342500000000001</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
@@ -1680,35 +1710,41 @@
       <c r="C4" s="4">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F4" s="4">
+      <c r="H4" s="4">
         <v>56.465794000000002</v>
       </c>
-      <c r="G4" s="4">
+      <c r="I4" s="4">
         <v>-3.12696</v>
       </c>
-      <c r="H4" s="4">
+      <c r="J4" s="4">
         <v>98.1</v>
       </c>
-      <c r="I4" s="4">
+      <c r="K4" s="4">
         <v>5.6565000000000003</v>
       </c>
-      <c r="J4" s="4">
-        <v>1</v>
-      </c>
-      <c r="K4" s="4">
+      <c r="L4" s="4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="4">
         <v>10.432399999999999</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
@@ -1718,35 +1754,41 @@
       <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="4">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F5" s="4">
+      <c r="H5" s="4">
         <v>56.468415</v>
       </c>
-      <c r="G5" s="4">
+      <c r="I5" s="4">
         <v>-3.1256499999999998</v>
       </c>
-      <c r="H5" s="4">
+      <c r="J5" s="4">
         <v>76.5</v>
       </c>
-      <c r="I5" s="4">
+      <c r="K5" s="4">
         <v>6.4452999999999996</v>
       </c>
-      <c r="J5" s="4">
+      <c r="L5" s="4">
         <v>2</v>
       </c>
-      <c r="K5" s="4">
+      <c r="M5" s="4">
         <v>9.4054000000000002</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
@@ -1756,33 +1798,39 @@
       <c r="C6" s="4">
         <v>1</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="4">
+      <c r="H6" s="4">
         <v>56.470269999999999</v>
       </c>
-      <c r="G6" s="4">
+      <c r="I6" s="4">
         <v>-3.1406999999999998</v>
       </c>
-      <c r="H6" s="4">
+      <c r="J6" s="4">
         <v>76.2</v>
       </c>
-      <c r="I6" s="4">
+      <c r="K6" s="4">
         <v>16.232500000000002</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4">
+      <c r="L6" s="4"/>
+      <c r="M6" s="4">
         <v>21.435600000000001</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="N6" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>26</v>
       </c>
@@ -1792,33 +1840,39 @@
       <c r="C7" s="4">
         <v>2</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="4">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F7" s="4">
+      <c r="H7" s="4">
         <v>56.471969000000001</v>
       </c>
-      <c r="G7" s="4">
+      <c r="I7" s="4">
         <v>-3.11985</v>
       </c>
-      <c r="H7" s="4">
+      <c r="J7" s="4">
         <v>62.4</v>
       </c>
-      <c r="I7" s="4">
+      <c r="K7" s="4">
         <v>17.552600000000002</v>
       </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4">
+      <c r="L7" s="4"/>
+      <c r="M7" s="4">
         <v>22.467400000000001</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="N7" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
@@ -1828,35 +1882,41 @@
       <c r="C8" s="4">
         <v>1</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="4">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F8" s="4">
+      <c r="H8" s="4">
         <v>56.468760000000003</v>
       </c>
-      <c r="G8" s="4">
+      <c r="I8" s="4">
         <v>-3.1153</v>
       </c>
-      <c r="H8" s="4">
+      <c r="J8" s="4">
         <v>56.4</v>
       </c>
-      <c r="I8" s="4">
+      <c r="K8" s="4">
         <v>4.5321999999999996</v>
       </c>
-      <c r="J8" s="4">
+      <c r="L8" s="4">
         <v>2</v>
       </c>
-      <c r="K8" s="4">
+      <c r="M8" s="4">
         <v>16.546600000000002</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="N8" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
@@ -1866,35 +1926,41 @@
       <c r="C9" s="4">
         <v>2</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="4">
+        <v>4</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F9" s="4">
+      <c r="H9" s="4">
         <v>56.467841999999997</v>
       </c>
-      <c r="G9" s="4">
+      <c r="I9" s="4">
         <v>-3.1088</v>
       </c>
-      <c r="H9" s="4">
+      <c r="J9" s="4">
         <v>68.900000000000006</v>
       </c>
-      <c r="I9" s="4">
+      <c r="K9" s="4">
         <v>6.3562000000000003</v>
       </c>
-      <c r="J9" s="4">
+      <c r="L9" s="4">
         <v>3</v>
       </c>
-      <c r="K9" s="4">
+      <c r="M9" s="4">
         <v>15.545299999999999</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="N9" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1904,35 +1970,41 @@
       <c r="C10" s="4">
         <v>1</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>3</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F10" s="4">
+      <c r="H10" s="4">
         <v>56.469270999999999</v>
       </c>
-      <c r="G10" s="4">
+      <c r="I10" s="4">
         <v>-3.14317</v>
       </c>
-      <c r="H10" s="4">
+      <c r="J10" s="4">
         <v>85.6</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>14.5463</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>6</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>24.545300000000001</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="N10" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -1942,35 +2014,41 @@
       <c r="C11" s="4">
         <v>2</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F11" s="4">
+      <c r="H11" s="4">
         <v>56.472653000000001</v>
       </c>
-      <c r="G11" s="4">
+      <c r="I11" s="4">
         <v>-3.1432699999999998</v>
       </c>
-      <c r="H11" s="4">
+      <c r="J11" s="4">
         <v>23.6</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>20.435600000000001</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>8</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>25.5366</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="N11" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
@@ -1980,28 +2058,34 @@
       <c r="C12" s="4">
         <v>1</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="4">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4">
+        <v>3</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F12" s="4">
+      <c r="H12" s="4">
         <v>56.461801000000001</v>
       </c>
-      <c r="G12" s="4">
+      <c r="I12" s="4">
         <v>-3.1385399999999999</v>
       </c>
-      <c r="H12" s="4">
+      <c r="J12" s="4">
         <v>85.9</v>
       </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12">
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
         <v>9.4344999999999999</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="N12" s="4" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2598,7 +2682,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2 D2">
-    <cfRule type="containsBlanks" dxfId="18" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2625,22 +2709,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="9" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>7</v>
       </c>
@@ -2651,79 +2740,85 @@
         <v>97</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>91</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>71</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>72</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsBlanks" dxfId="17" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2740,21 +2835,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -2765,29 +2866,35 @@
         <v>97</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>91</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>71</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>72</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
   </sheetData>
   <dataValidations xWindow="96" yWindow="450" count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Same format as the &quot;DATA&quot; sheet, but this time the recording date goes into the matrix cells. Dates should be formatted according to the &quot;ACQDATE&quot; field of the MCPD." sqref="A1:D1" xr:uid="{13E30841-E8AE-4AEA-9BB5-750247107F69}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please enter data here!" prompt="Same format as the &quot;DATA&quot; sheet, but this time the recording date goes into the matrix cells. Dates should be formatted according to the &quot;ACQDATE&quot; field of the MCPD." sqref="A1:F1" xr:uid="{13E30841-E8AE-4AEA-9BB5-750247107F69}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>